<commit_message>
hopefully fixed fixed security issues
</commit_message>
<xml_diff>
--- a/www/excelReport.xlsx
+++ b/www/excelReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>&lt;html&gt;&lt;head&gt;&lt;meta http-equiv="Content-Type" content="text/html; charset=utf-8"&gt;&lt;/head&gt;&lt;body style="word-wrap: break-word; -webkit-nbsp-mode: space; line-break: after-white-space;" class=""&gt;&lt;br class=""&gt;&lt;div&gt;&lt;br class=""&gt;&lt;blockquote type="cite" class=""&gt;&lt;div class=""&gt;Begin forwarded message:&lt;/div&gt;&lt;br class="Apple-interchange-newline"&gt;&lt;div style="margin-top: 0px; margin-right: 0px; margin-bottom: 0px; margin-left: 0px;" class=""&gt;&lt;span style="font-family: -webkit-system-font, Helvetica Neue, Helvetica, sans-serif; color:rgba(0, 0, 0, 1.0);" class=""&gt;&lt;b class=""&gt;From: &lt;/b&gt;&lt;/span&gt;&lt;span style="font-family: -webkit-system-font, Helvetica Neue, Helvetica, sans-serif;" class=""&gt;Ana Mattuzzi-Stojanović &amp;lt;&lt;a href="mailto:ana.mattuzzi@me.com" class=""&gt;ana.mattuzzi@me.com&lt;/a&gt;&amp;gt;&lt;br class=""&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="margin-top: 0px; margin-right: 0px; margin-bottom: 0px; margin-left: 0px;" class=""&gt;&lt;span style="font-family: -webkit-system-font, Helvetica Neue, Helvetica, sans-serif; color:rgba(0, 0, 0, 1.0);" class=""&gt;&lt;b class=""&gt;Subject: &lt;/b&gt;&lt;/span&gt;&lt;span style="font-family: -webkit-system-font, Helvetica Neue, Helvetica, sans-serif;" class=""&gt;&lt;b class=""&gt;This is the first email I should send&lt;/b&gt;&lt;br class=""&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="margin-top: 0px; margin-right: 0px; margin-bottom: 0px; margin-left: 0px;" class=""&gt;&lt;span style="font-family: -webkit-system-font, Helvetica Neue, Helvetica, sans-serif; color:rgba(0, 0, 0, 1.0);" class=""&gt;&lt;b class=""&gt;Date: &lt;/b&gt;&lt;/span&gt;&lt;span style="font-family: -webkit-system-font, Helvetica Neue, Helvetica, sans-serif;" class=""&gt;January 26, 2019 at 12:39:38 PM GMT+1&lt;br class=""&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="margin-top: 0px; margin-right: 0px; margin-bottom: 0px; margin-left: 0px;" class=""&gt;&lt;span style="font-family: -webkit-system-font, Helvetica Neue, Helvetica, sans-serif; color:rgba(0, 0, 0, 1.0);" class=""&gt;&lt;b class=""&gt;To: &lt;/b&gt;&lt;/span&gt;&lt;span style="font-family: -webkit-system-font, Helvetica Neue, Helvetica, sans-serif;" class=""&gt;&lt;a href="mailto:smbaiwsy@gmail.com" class=""&gt;smbaiwsy@gmail.com&lt;/a&gt;&lt;br class=""&gt;&lt;/span&gt;&lt;/div&gt;&lt;br class=""&gt;&lt;div class=""&gt;&lt;div class=""&gt;I am sending the attachments, as well.&lt;br class=""&gt;Cheers,&lt;br class=""&gt;Ana&lt;br class=""&gt;&lt;/div&gt;&lt;/div&gt;&lt;/blockquote&gt;&lt;/div&gt;&lt;/body&gt;&lt;/html&gt;&lt;a href='files/pdf/products-engineering-en-20181219.pdf' target='_blank'&gt;products-engineering-en-20181219&lt;/a&gt;&lt;br /&gt;</t>
   </si>
@@ -27,6 +27,21 @@
   </si>
   <si>
     <t>&lt;html&gt;&lt;head&gt;&lt;meta http-equiv="Content-Type" content="text/html; charset=utf-8"&gt;&lt;/head&gt;&lt;body style="word-wrap: break-word; -webkit-nbsp-mode: space; line-break: after-white-space;" class=""&gt;&lt;br class=""&gt;&lt;div&gt;&lt;br class=""&gt;&lt;blockquote type="cite" class=""&gt;&lt;div class=""&gt;Begin forwarded message:&lt;/div&gt;&lt;br class="Apple-interchange-newline"&gt;&lt;div style="margin-top: 0px; margin-right: 0px; margin-bottom: 0px; margin-left: 0px;" class=""&gt;&lt;span style="font-family: -webkit-system-font, Helvetica Neue, Helvetica, sans-serif; color:rgba(0, 0, 0, 1.0);" class=""&gt;&lt;b class=""&gt;From: &lt;/b&gt;&lt;/span&gt;&lt;span style="font-family: -webkit-system-font, Helvetica Neue, Helvetica, sans-serif;" class=""&gt;Kathy Caprino &amp;lt;&lt;a href="mailto:kathy@kathycaprino.com" class=""&gt;kathy@kathycaprino.com&lt;/a&gt;&amp;gt;&lt;br class=""&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="margin-top: 0px; margin-right: 0px; margin-bottom: 0px; margin-left: 0px;" class=""&gt;&lt;span style="font-family: -webkit-system-font, Helvetica Neue, Helvetica, sans-serif; color:rgba(0, 0, 0, 1.0);" class=""&gt;&lt;b class=""&gt;Subject: &lt;/b&gt;&lt;/span&gt;&lt;span style="font-family: -webkit-system-font, Helvetica Neue, Helvetica, sans-serif;" class=""&gt;&lt;b class=""&gt;LAST CHANCE to transform your career with Kathy in the Amazing Career Project course&lt;/b&gt;&lt;br class=""&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="margin-top: 0px; margin-right: 0px; margin-bottom: 0px; margin-left: 0px;" class=""&gt;&lt;span style="font-family: -webkit-system-font, Helvetica Neue, Helvetica, sans-serif; color:rgba(0, 0, 0, 1.0);" class=""&gt;&lt;b class=""&gt;Date: &lt;/b&gt;&lt;/span&gt;&lt;span style="font-family: -webkit-system-font, Helvetica Neue, Helvetica, sans-serif;" class=""&gt;January 26, 2019 at 2:21:31 PM GMT+1&lt;br class=""&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="margin-top: 0px; margin-right: 0px; margin-bottom: 0px; margin-left: 0px;" class=""&gt;&lt;span style="font-family: -webkit-system-font, Helvetica Neue, Helvetica, sans-serif; color:rgba(0, 0, 0, 1.0);" class=""&gt;&lt;b class=""&gt;To: &lt;/b&gt;&lt;/span&gt;&lt;span style="font-family: -webkit-system-font, Helvetica Neue, Helvetica, sans-serif;" class=""&gt;&lt;a href="mailto:ana.mattuzzi@me.com" class=""&gt;ana.mattuzzi@me.com&lt;/a&gt;&lt;br class=""&gt;&lt;/span&gt;&lt;/div&gt;&lt;br class=""&gt;&lt;div class=""&gt;&lt;div style="caret-color: rgb(0, 0, 0); font-family: Helvetica; font-size: 12px; font-style: normal; font-variant-caps: normal; font-weight: normal; letter-spacing: normal; text-align: start; text-indent: 0px; text-transform: none; white-space: normal; word-spacing: 0px; -webkit-text-stroke-width: 0px; background-color: rgb(255, 255, 255); text-decoration: none;" class=""&gt;&lt;div style="max-width: 600px; background-image: none; background-attachment: scroll; background-color: rgb(255, 255, 255); margin: 0px auto; background-position: 0% 0%; background-repeat: repeat repeat;" class=""&gt;&lt;table cellspacing="0" cellpadding="0" border="0" align="center" style="border-collapse: collapse; font-size: 0px; width: 600px; background-image: none; background-attachment: scroll; background-color: rgb(255, 255, 255); background-position: 0% 0%; background-repeat: repeat repeat;" class=""&gt;&lt;tbody class=""&gt;&lt;tr class=""&gt;&lt;td style="border-collapse: collapse; text-align: center; vertical-align: top; font-size: 0px;" class=""&gt;&lt;div class="column-100 column" style="text-align: left; vertical-align: top; display: inline-block; width: 600px;"&gt;&lt;table width="100%" cellspacing="0" cellpadding="0" border="0" style="border-collapse: collapse;" class=""&gt;&lt;tbody class=""&gt;&lt;tr class=""&gt;&lt;td class="alignmentContainer" style="border-collapse: collapse; overflow-wrap: break-word; font-size: 0px; padding: 0px; text-align: center;"&gt;&lt;div style="padding-top: 15px;" class=""&gt;&amp;nbsp;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/div&gt;&lt;div style="max-width: 600px; background-image: none; background-attachment: scroll; background-color: rgb(255, 255, 255); margin: 0px auto; background-position: 0% 0%; background-repeat: repeat repeat;" class=""&gt;&lt;table cellspacing="0" cellpadding="0" border="0" align="center" style="border-collapse: collapse; font-size: 0px; width: 600px; background-image: none; background-attachment: scroll; background-color: rgb(255, 255, 255); background-position: 0% 0%; background-repeat: repeat repeat;" class=""&gt;&lt;tbody class=""&gt;&lt;tr class=""&gt;&lt;td style="border-collapse: collapse; text-align: center; vertical-align: top; font-size: 0px;" class=""&gt;&lt;div class="column-100 column" style="text-align: left; vertical-align: top; display: inline-block; width: 600px;"&gt;&lt;table width="100%" cellspacing="0" cellpadding="0" border="0" style="border-collapse: collapse;" class=""&gt;&lt;tbody class=""&gt;&lt;tr class=""&gt;&lt;td style="border-collapse: collapse; overflow-wrap: break-word; font-size: 0px; padding: 15px; text-align: left;" class=""&gt;&lt;div class=""&gt;&lt;p class="style-scope bard-text-block" style="font-family: Helvetica, Arial, sans-serif; font-size: 14px; padding: 0px; margin: 0px 0px 13px; line-height: 1.6;"&gt;Dear Ana Mattuzzi,&lt;/p&gt;&lt;p class="style-scope bard-text-block" style="font-family: Helvetica, Arial, sans-serif; font-size: 14px; padding: 0px; margin: 13px 0px; line-height: 1.6;"&gt;&lt;b class="style-scope bard-text-block" style="padding: 0px; line-height: 1.6;"&gt;Just a quick note that this is your absolute LAST CHANCE to work with me to transform your work and your life in the Amazing Career Project online course. Enrollment closes Sunday night! And this course won’t be available again for months.&lt;/b&gt;&lt;/p&gt;&lt;p class="style-scope bard-text-block" style="font-family: Helvetica, Arial, sans-serif; font-size: 14px; padding: 0px; margin: 13px 0px; line-height: 1.6;"&gt;If you’ve been scratching your head wondering why you just won’t pull the trigger, let’s change that for you. Sign up before the window closes for good at&lt;span class="Apple-converted-space"&gt;&amp;nbsp;&lt;/span&gt;&lt;b class="style-scope bard-text-block" style="padding: 0px; line-height: 1.6;"&gt;midnight EST Sunday&lt;/b&gt;!&lt;/p&gt;&lt;p class="style-scope bard-text-block" style="font-family: Helvetica, Arial, sans-serif; font-size: 14px; padding: 0px; margin: 13px 0px; line-height: 1.6;"&gt;If you want not only expert support from me, but an amazing international community of like-minded, inspiring women to help you on your journey to career growth, this is BEST place!&lt;/p&gt;&lt;p class="style-scope bard-text-block" style="font-family: Helvetica, Arial, sans-serif; font-size: 14px; padding: 0px; margin: 13px 0px; line-height: 1.6;"&gt;Visit my&lt;span class="Apple-converted-space"&gt;&amp;nbsp;&lt;/span&gt;&lt;a class="style-scope bard-text-block" href="https://is-tracking-link-api-prod.appspot.com/api/v1/click/6633533005103104/6008624757342208" target="_blank" style="color: rgb(44, 132, 138); padding: 0px; line-height: 1.6;"&gt;Amazing Career Project&lt;/a&gt;&lt;span class="Apple-converted-space"&gt;&amp;nbsp;&lt;/span&gt;page to learn what other course members have said about working with me, and both the hoped-for AND unexpected benefits they received!&lt;/p&gt;&lt;p class="style-scope bard-text-block" style="font-family: Helvetica, Arial, sans-serif; font-size: 14px; padding: 0px; margin: 13px 0px; line-height: 1.6;"&gt;&lt;i class="style-scope bard-text-block" style="padding: 0px; line-height: 1.6;"&gt;The Amazing Career Project&lt;/i&gt;&lt;span class="Apple-converted-space"&gt;&amp;nbsp;&lt;/span&gt;is truly the only program of its kind that incorporates powerful therapeutic principles, career coaching strategies, AND personal growth training all in one,&lt;span class="Apple-converted-space"&gt;&amp;nbsp;&lt;/span&gt;&lt;i class="style-scope bard-text-block" style="padding: 0px; line-height: 1.6;"&gt;within a beautiful supportive group format&lt;/i&gt;.&lt;span class="Apple-converted-space"&gt;&amp;nbsp;&lt;/span&gt;&lt;/p&gt;&lt;p class="style-scope bard-text-block" style="font-family: Helvetica, Arial, sans-serif; font-size: 14px; padding: 0px; margin: 13px 0px; line-height: 1.6;"&gt;I share everything I’ve learned throughout 13 years or career and life transformation work with over 13,000 women about the 5 most critical phases you need to engage in, to successfully build a thrilling life and career that you’ll love and feel proud of each and every day.&lt;/p&gt;&lt;p class="style-scope bard-text-block" style="font-family: Helvetica, Arial, sans-serif; font-size: 14px; padding: 0px; margin: 13px 0px; line-height: 1.6;"&gt;&lt;b class="style-scope bard-text-block" style="padding: 0px; line-height: 1.6;"&gt;Beginning February 4th, you’ll work with me (and an amazing group of course members) in a transformative 16-week course that gives you:&lt;/b&gt;&lt;/p&gt;&lt;p class="style-scope bard-text-block" style="font-family: Helvetica, Arial, sans-serif; font-size: 14px; padding: 0px; margin: 13px 0px; line-height: 1.6;"&gt;- 16 video training modules that teach the 16 most essential steps to dramatically transforming your personal and professional life, in as little as 16 weeks&lt;/p&gt;&lt;p class="style-scope bard-text-block" style="font-family: Helvetica, Arial, sans-serif; font-size: 14px; padding: 0px; margin: 13px 0px; line-height: 1.6;"&gt;- 16 powerful homework assignments that help you move forward and take the action you need to to build more happiness and success&lt;/p&gt;&lt;p class="style-scope bard-text-block" style="font-family: Helvetica, Arial, sans-serif; font-size: 14px; padding: 0px; margin: 13px 0px; line-height: 1.6;"&gt;- 16 weekly open “Office Hour” group calls with me to get direct coaching on your questions and challenges&lt;/p&gt;&lt;p class="style-scope bard-text-block" style="font-family: Helvetica, Arial, sans-serif; font-size: 14px; padding: 0px; margin: 13px 0px; line-height: 1.6;"&gt;- A hand-picked expert collection of premier resources for additional support and learning&lt;/p&gt;&lt;p class="style-scope bard-text-block" style="font-family: Helvetica, Arial, sans-serif; font-size: 14px; padding: 0px; margin: 13px 0px; line-height: 1.6;"&gt;- A fantastic online support network and empowering community for all attendees&lt;/p&gt;&lt;p class="style-scope bard-text-block" style="font-family: Helvetica, Arial, sans-serif; font-size: 14px; padding: 0px; margin: 13px 0px; line-height: 1.6;"&gt;- Lifetime 20% Discount (and insider special offers) to my private coaching and other programs, for additional, hands-on support and special events&lt;/p&gt;&lt;p class="style-scope bard-text-block" style="font-family: Helvetica, Arial, sans-serif; font-size: 14px; padding: 0px; margin: 13px 0px; line-height: 1.6;"&gt;- Access to a special post-program group for course graduates, to continue the learning, encourage and motivation&lt;/p&gt;&lt;p class="style-scope bard-text-block" style="font-family: Helvetica, Arial, sans-serif; font-size: 14px; padding: 0px; margin: 13px 0px; line-height: 1.6;"&gt;...all aimed to help you finally break through your inertia and dissatisfaction with your personal and professional life, to feeling like you're doing work you're meant to, with people you love and respect, while balancing your life outside of work in ways that make you happy.&lt;/p&gt;&lt;p class="style-scope bard-text-block" style="font-family: Helvetica, Arial, sans-serif; font-size: 14px; padding: 0px; margin: 13px 0px; line-height: 1.6;"&gt;If you’re ready for more growth, joy and reward, register today.&lt;span class="Apple-converted-space"&gt;&amp;nbsp;&lt;/span&gt;&lt;br class=""&gt;&lt;/p&gt;&lt;p class="style-scope bard-text-block" style="font-family: Helvetica, Arial, sans-serif; font-size: 14px; padding: 0px; margin: 13px 0px; line-height: 1.6;"&gt;&lt;a href="https://is-tracking-link-api-prod.appspot.com/api/v1/click/4872225704378368/6008624757342208" class="style-scope bard-text-block" target="_blank" style="color: rgb(44, 132, 138); padding: 0px; line-height: 1.6;"&gt;&lt;b class="style-scope bard-text-block" style="padding: 0px; line-height: 1.6;"&gt;SO GO AHEAD, TAKE YOUR TICKET TO LIFE CHANGE TODAY.&lt;/b&gt;&lt;/a&gt;&lt;br class=""&gt;&lt;/p&gt;&lt;p class="style-scope bard-text-block" style="font-family: Helvetica, Arial, sans-serif; font-size: 14px; padding: 0px; margin: 13px 0px; line-height: 1.6;"&gt;See on you February 4th, and I’m sending all my love and best wishes for an amazing new chapter in your life and work!&lt;/p&gt;&lt;p class="style-scope bard-text-block" style="font-family: Helvetica, Arial, sans-serif; font-size: 14px; padding: 0px; margin: 13px 0px; line-height: 1.6;"&gt;Kathy&lt;br class=""&gt;&lt;br class=""&gt;&lt;/p&gt;&lt;p class="style-scope bard-text-block" style="font-family: Helvetica, Arial, sans-serif; font-size: 14px; padding: 0px; margin: 13px 0px; line-height: 1.6;"&gt;P.S. Don’t be one of those people who stays stuck in unhappiness, and uses&lt;span class="Apple-converted-space"&gt;&amp;nbsp;&lt;/span&gt;&lt;a href="https://is-tracking-link-api-prod.appspot.com/api/v1/click/6076154161135616/6008624757342208" class="style-scope bard-text-block" target="_blank" style="color: rgb(44, 132, 138); padding: 0px; line-height: 1.6;"&gt;these 8 common and damaging excuses&lt;/a&gt;&lt;span class="Apple-converted-space"&gt;&amp;nbsp;&lt;/span&gt;NOT to move forward. Take the leap!&lt;/p&gt;&lt;p class="style-scope bard-text-block" style="font-family: Helvetica, Arial, sans-serif; font-size: 14px; padding: 0px; margin: 13px 0px 0px; line-height: 1.6;"&gt;P.P.S. Do you know what your&lt;span class="Apple-converted-space"&gt;&amp;nbsp;&lt;/span&gt;&lt;b class="style-scope bard-text-block" style="padding: 0px; line-height: 1.6;"&gt;Dominant Action Style&lt;/b&gt;&lt;span class="Apple-converted-space"&gt;&amp;nbsp;&lt;/span&gt;is? If not, you’re limiting your happiness and success in both life and work.&lt;span class="Apple-converted-space"&gt;&amp;nbsp;&lt;/span&gt;&lt;a href="https://is-tracking-link-api-prod.appspot.com/api/v1/click/4971259764932608/6008624757342208" class="style-scope bard-text-block" target="_blank" style="color: rgb(44, 132, 138); padding: 0px; line-height: 1.6;"&gt;Click here to learn more&lt;/a&gt;, and join me beginning February 4th to learn to leverage -- and honor -- who you really are!&lt;span class="Apple-converted-space"&gt;&amp;nbsp;&lt;/span&gt;&lt;/p&gt;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/div&gt;&lt;div style="max-width: 600px; background-image: none; background-attachment: scroll; background-color: rgb(255, 255, 255); margin: 0px auto; background-position: 0% 0%; background-repeat: repeat repeat;" class=""&gt;&lt;table cellspacing="0" cellpadding="0" border="0" align="center" style="border-collapse: collapse; font-size: 0px; width: 600px; background-image: none; background-attachment: scroll; background-color: rgb(255, 255, 255); background-position: 0% 0%; background-repeat: repeat repeat;" class=""&gt;&lt;tbody class=""&gt;&lt;tr class=""&gt;&lt;td style="border-collapse: collapse; text-align: center; vertical-align: top; font-size: 0px;" class=""&gt;&lt;div class="column-100 column" style="text-align: left; vertical-align: top; display: inline-block; width: 600px;"&gt;&lt;table width="100%" cellspacing="0" cellpadding="0" border="0" style="border-collapse: collapse;" class=""&gt;&lt;tbody class=""&gt;&lt;tr class=""&gt;&lt;td class="alignmentContainer" style="border-collapse: collapse; overflow-wrap: break-word; font-size: 0px; padding: 15px; text-align: center;"&gt;&lt;div class=""&gt;&lt;div xmlns="http://www.w3.org/1999/xhtml" style="width: 427.5px; border-color: rgb(0, 0, 0); background-color: rgb(0, 0, 0); height: 1px; margin: 0px auto;" class=""&gt;&lt;/div&gt;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/div&gt;&lt;div style="max-width: 600px; background-image: none; background-attachment: scroll; background-color: rgb(255, 255, 255); margin: 0px auto; background-position: 0% 0%; background-repeat: repeat repeat;" class=""&gt;&lt;table cellspacing="0" cellpadding="0" border="0" align="center" style="border-collapse: collapse; font-size: 0px; width: 600px; background-image: none; background-attachment: scroll; background-color: rgb(255, 255, 255); background-position: 0% 0%; background-repeat: repeat repeat;" class=""&gt;&lt;tbody class=""&gt;&lt;tr class=""&gt;&lt;td style="border-collapse: collapse; text-align: center; vertical-align: top; font-size: 0px;" class=""&gt;&lt;div class="column-100 column" style="text-align: left; vertical-align: top; display: inline-block; width: 600px;"&gt;&lt;table width="100%" cellspacing="0" cellpadding="0" border="0" style="border-collapse: collapse;" class=""&gt;&lt;tbody class=""&gt;&lt;tr class=""&gt;&lt;td class="alignmentContainer" style="border-collapse: collapse; overflow-wrap: break-word; font-size: 0px; padding: 0px; text-align: center;"&gt;&lt;div style="padding-top: 15px;" class=""&gt;&amp;nbsp;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/div&gt;&lt;div style="max-width: 600px; background-image: none; background-attachment: scroll; background-color: rgb(255, 255, 255); margin: 0px auto; background-position: 0% 0%; background-repeat: repeat repeat;" class=""&gt;&lt;table cellspacing="0" cellpadding="0" border="0" align="center" style="border-collapse: collapse; font-size: 0px; width: 600px; background-image: none; background-attachment: scroll; background-color: rgb(255, 255, 255); background-position: 0% 0%; background-repeat: repeat repeat;" class=""&gt;&lt;tbody class=""&gt;&lt;tr class=""&gt;&lt;td style="border-collapse: collapse; text-align: center; vertical-align: top; font-size: 0px;" class=""&gt;&lt;div class="column-100 column" style="text-align: left; vertical-align: top; display: inline-block; width: 600px;"&gt;&lt;table width="100%" cellspacing="0" cellpadding="0" border="0" style="border-collapse: collapse;" class=""&gt;&lt;tbody class=""&gt;&lt;tr class=""&gt;&lt;td class="alignmentContainer" style="border-collapse: collapse; overflow-wrap: break-word; font-size: 0px; padding: 15px; text-align: center;"&gt;&lt;div style="margin-left: auto; margin-right: auto;" class=""&gt;&lt;p style="font-family: Helvetica, Arial, sans-serif; padding: 0px; margin: 0px 0px 13px; line-height: 1.6; color: rgb(153, 153, 153); font-size: 11px;" class=""&gt;Having trouble viewing this email?&lt;span class="Apple-converted-space"&gt;&amp;nbsp;&lt;/span&gt;&lt;a href="https://yj234.infusionsoft.com/app/hostedEmail/35441689/fb4d722ac5fa2907" target="_blank" class=""&gt;Click here&lt;/a&gt;&lt;/p&gt;&lt;p style="font-family: Helvetica, Arial, sans-serif; padding: 0px; margin: 13px 0px; line-height: 1.6; color: rgb(153, 153, 153); font-size: 11px;" class=""&gt;&lt;a href="https://yj234.infusionsoft.com/app/linkClick/32975/f3fdf0af6aea14c6/35441689/fb4d722ac5fa2907" target="_blank" style="text-decoration: underline; padding: 0px; line-height: 1.6; color: rgb(153, 153, 153);" class=""&gt;Unsubscribe&lt;/a&gt;&lt;/p&gt;&lt;p style="font-family: Helvetica, Arial, sans-serif; padding: 0px; margin: 13px 0px 0px; line-height: 1.6; color: rgb(153, 153, 153); font-size: 11px;" class=""&gt;Ellia Communications P.O. Box 302 Wilton, Connecticut 06897 United States&lt;/p&gt;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/div&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;/div&gt;&lt;/div&gt;&lt;img src="https://is-tracking-pixel-api-prod.appspot.com/api/v1/render/5237588427014144/5223636388544512" width="1" height="1" border="0" alt="" style="border: 0px; height: auto; line-height: 12px; outline: none; text-decoration: none; caret-color: rgb(0, 0, 0); font-family: Helvetica; font-size: 12px; font-style: normal; font-variant-caps: normal; font-weight: normal; letter-spacing: normal; text-align: start; text-indent: 0px; text-transform: none; white-space: normal; word-spacing: 0px; -webkit-text-stroke-width: 0px; background-color: rgb(255, 255, 255);" class=""&gt;&lt;span style="caret-color: rgb(0, 0, 0); font-family: Helvetica; font-size: 12px; font-style: normal; font-variant-caps: normal; font-weight: normal; letter-spacing: normal; text-align: start; text-indent: 0px; text-transform: none; white-space: normal; word-spacing: 0px; -webkit-text-stroke-width: 0px; background-color: rgb(255, 255, 255); text-decoration: none; float: none; display: inline !important;" class=""&gt;&lt;/span&gt;&lt;/div&gt;&lt;/blockquote&gt;&lt;/div&gt;&lt;br class=""&gt;&lt;/body&gt;&lt;/html&gt;</t>
+  </si>
+  <si>
+    <t>&lt;html&gt;&lt;head&gt;&lt;meta http-equiv="Content-Type" content="text/html; charset=utf-8"&gt;&lt;/head&gt;&lt;body style="word-wrap: break-word; -webkit-nbsp-mode: space; line-break: after-white-space;" class=""&gt;&lt;br class=""&gt;&lt;div&gt;&lt;br class=""&gt;&lt;blockquote type="cite" class=""&gt;&lt;div class=""&gt;Begin forwarded message:&lt;/div&gt;&lt;br class="Apple-interchange-newline"&gt;&lt;div style="margin-top: 0px; margin-right: 0px; margin-bottom: 0px; margin-left: 0px;" class=""&gt;&lt;span style="font-family: -webkit-system-font, Helvetica Neue, Helvetica, sans-serif; color:rgba(0, 0, 0, 1.0);" class=""&gt;&lt;b class=""&gt;From: &lt;/b&gt;&lt;/span&gt;&lt;span style="font-family: -webkit-system-font, Helvetica Neue, Helvetica, sans-serif;" class=""&gt;Kiefer &amp;lt;&lt;a href="mailto:kiefer@carbbackloading.com" class=""&gt;kiefer@carbbackloading.com&lt;/a&gt;&amp;gt;&lt;br class=""&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="margin-top: 0px; margin-right: 0px; margin-bottom: 0px; margin-left: 0px;" class=""&gt;&lt;span style="font-family: -webkit-system-font, Helvetica Neue, Helvetica, sans-serif; color:rgba(0, 0, 0, 1.0);" class=""&gt;&lt;b class=""&gt;Subject: &lt;/b&gt;&lt;/span&gt;&lt;span style="font-family: -webkit-system-font, Helvetica Neue, Helvetica, sans-serif;" class=""&gt;&lt;b class=""&gt;How To “Turn On” Happy Hormones&lt;/b&gt;&lt;br class=""&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="margin-top: 0px; margin-right: 0px; margin-bottom: 0px; margin-left: 0px;" class=""&gt;&lt;span style="font-family: -webkit-system-font, Helvetica Neue, Helvetica, sans-serif; color:rgba(0, 0, 0, 1.0);" class=""&gt;&lt;b class=""&gt;Date: &lt;/b&gt;&lt;/span&gt;&lt;span style="font-family: -webkit-system-font, Helvetica Neue, Helvetica, sans-serif;" class=""&gt;January 26, 2019 at 8:30:03 AM GMT+1&lt;br class=""&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="margin-top: 0px; margin-right: 0px; margin-bottom: 0px; margin-left: 0px;" class=""&gt;&lt;span style="font-family: -webkit-system-font, Helvetica Neue, Helvetica, sans-serif; color:rgba(0, 0, 0, 1.0);" class=""&gt;&lt;b class=""&gt;To: &lt;/b&gt;&lt;/span&gt;&lt;span style="font-family: -webkit-system-font, Helvetica Neue, Helvetica, sans-serif;" class=""&gt;Ana Mattuzzi &amp;lt;&lt;a href="mailto:ana.mattuzzi@me.com" class=""&gt;ana.mattuzzi@me.com&lt;/a&gt;&amp;gt;&lt;br class=""&gt;&lt;/span&gt;&lt;/div&gt;&lt;br class=""&gt;&lt;div class=""&gt;&lt;table align="center" border="0" cellpadding="0" cellspacing="0" id="emailContainer" width="100%" style="caret-color: rgb(0, 0, 0); font-family: Helvetica; font-size: 12px; font-style: normal; font-variant-caps: normal; font-weight: normal; letter-spacing: normal; text-align: start; text-indent: 0px; text-transform: none; white-space: normal; word-spacing: 0px; -webkit-text-stroke-width: 0px; text-decoration: none;" class=""&gt;&lt;tbody class=""&gt;&lt;tr class=""&gt;&lt;td align="left" valign="top" style="display: block; max-width: 490px; background-color: rgb(255, 255, 255); font-family: georgia, serif; -webkit-font-smoothing: antialiased; font-size: 18px; line-height: 25px;" class=""&gt;&lt;p class=""&gt;Have you ever had nervous thoughts, constant worry or just a sense of hopelessness? + +&lt;/p&gt;&lt;p class=""&gt;I have to admit, I’ve experienced some anxiety and depression here and there throughout my life.&amp;nbsp;&lt;/p&gt;&lt;p class=""&gt;&lt;em class=""&gt;It’s a crippling feeling. + +&lt;/em&gt;&lt;/p&gt;&lt;p class=""&gt;Right now, about 1 in 4 adults suffer from a mood disorder.&amp;nbsp;&lt;/p&gt;&lt;p class=""&gt;&lt;u class=""&gt;Anxiety effects 40 million Americans and Depression is now a leading disability worldwide.&lt;/u&gt;&lt;/p&gt;&lt;p class=""&gt; + +Numerous studies have found that people with anxiety and depression have high levels of systemic inflammation, an over-reactive stress response and an unhealthy micro-biome. +&lt;/p&gt;&lt;p class=""&gt;&lt;em class=""&gt;Did you know that your gut microbes determine the availability of essential building blocks for our&amp;nbsp;feel-good hormone, serotonin? + +&lt;/em&gt;&lt;/p&gt;&lt;p class=""&gt;When we have a specific species of bacteria in our micro-biome we’ll have&amp;nbsp;increasing levels of tryptophan. + +&lt;/p&gt;&lt;p class=""&gt;This little molecule is converted directly into serotonin, and could be called the happiness-molecule. Less tryptophan means less serotonin, and less serotonin means less happiness.  +&lt;/p&gt;&lt;p class=""&gt;By having the correct species of bacteria in our micro-biome not only do we increase tryptophan but the micro-biome shields it from being destroyed.&lt;/p&gt;&lt;p class=""&gt;That’s just one of the many reasons I developed&lt;span class="Apple-converted-space"&gt;&amp;nbsp;&lt;/span&gt;&lt;a href="http://superhuman-llc.trk.klaviyomail.com/wf/click?upn=zmuOzL36mrVVmT72mbCegs28rLCRmWW61D4cjGIPwYnrbB9q4iJS822erjraxJmy1Tvueu5H2InlHGLZS6zsotvLofnu7zjgclLtfXppE1-2Bun9JuflB50cqgb8Fsbf79TJxWMlL9ux8Eq34cs7bujnu8Xtv4PaylVl-2B1bq7PkeoUbfGvJZxjFbmmVfa4Da93_Texcm7ClNCJnC4QA2ERJLXnpP159NPpcVDN41ujPpklaX56IaargMptC5MvyTMihfxX9YiA0F05gPp5qdOMRMkmCdrYpCx191z0byymYYeRIBF5yTWSN5nmLQxnnvmnPNGevdqmI3q-2FSqPr7GTSXv9I-2Flrjb26fvAnBOu9GsUbwgex-2FA9TOLfboLoMuW-2Bmr5OQydIj3BwS8J-2BY4ca6-2FGBH7j3OE7CSichVWhk3VStRaSmsxAzcKpWIk5KyCt4HvFM7WQ-2FVVFgLuYCVNFMSsZ5bz7dTePC9ALjQuvV7Je41A2e95d2-2B98j8GXzrmWyxi1kAI32R7g2q6laSUHcWa1FauHAss7lQV8AZJPnxH06iDluSXN2TTGVHLqub1EnTc8iac1UxKzS265Axyy4f83BQ-3D-3D" class=""&gt;Gut Shield&lt;/a&gt;.&lt;/p&gt;&lt;p class=""&gt;I put my heart and soul into the research uncovering which enzymes and bacteria strains would strengthen the immune system, lower inflammation, protect against food sensitivities and help activate “lean” genes.&lt;/p&gt;&lt;p class=""&gt;&lt;a href="http://superhuman-llc.trk.klaviyomail.com/wf/click?upn=r0bPYyJA929qYRDToey7d3to5wO0yahPabR7r-2BU4FVj8PahdYoLGk1q6dhfD07q3MsqJ4Y9eE8mHQ3frzhhklN-2FzbHfGDd4Wl5IJ82qYXYzGukWrjQNdxEtXT9ATSrKIqliFG3E9p0feuXi20Hna8fLXM3DMWK4n6vth28-2B4PYDSN1F38dQNXzOnIvAAAAau_Texcm7ClNCJnC4QA2ERJLXnpP159NPpcVDN41ujPpklaX56IaargMptC5MvyTMihfxX9YiA0F05gPp5qdOMRMkmCdrYpCx191z0byymYYeRIBF5yTWSN5nmLQxnnvmnPNGevdqmI3q-2FSqPr7GTSXv9I-2Flrjb26fvAnBOu9GsUbwgex-2FA9TOLfboLoMuW-2Bmr5OQydIj3BwS8J-2BY4ca6-2FGBNDluLXmO6O4Um-2BFJrmFcLLON-2BAYlz0Cm1I7X14LW1x7YNN8P2AmWlZrR5Sfm11RrTktAq42pAq-2BKprKeBamdcnSD32iKl8hogrUhUi-2BcXchhFARwx2o1t75u1-2FLW0ucKeMrmFfrGFsorwUSmNBGokg0LpKcxtttfYSdyzYUBt-2BCqGjPTqZGipL9Os2BVOqSPQ-3D-3D" class=""&gt;Get your supply here.&lt;span class="Apple-converted-space"&gt;&amp;nbsp;&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;&lt;p class=""&gt;Kiefer&lt;/p&gt;&lt;p class=""&gt;&lt;em class=""&gt;P.S. Did you see the new lower pricing?&amp;nbsp;&lt;a href="http://superhuman-llc.trk.klaviyomail.com/wf/click?upn=zmuOzL36mrVVmT72mbCegs28rLCRmWW61D4cjGIPwYnrbB9q4iJS822erjraxJmy1Tvueu5H2InlHGLZS6zsotvLofnu7zjgclLtfXppE1-2Bun9JuflB50cqgb8Fsbf79TJxWMlL9ux8Eq34cs7bujnu8Xtv4PaylVl-2B1bq7PkeoUbfGvJZxjFbmmVfa4Da93_Texcm7ClNCJnC4QA2ERJLXnpP159NPpcVDN41ujPpklaX56IaargMptC5MvyTMihfxX9YiA0F05gPp5qdOMRMkmCdrYpCx191z0byymYYeRIBF5yTWSN5nmLQxnnvmnPNGevdqmI3q-2FSqPr7GTSXv9I-2Flrjb26fvAnBOu9GsUbwgex-2FA9TOLfboLoMuW-2Bmr5OQydIj3BwS8J-2BY4ca6-2FGBIl7bekJL18-2F-2BjY0rJnn1hKPVldzEOEe99IlHJ3vkH1GdLA45GVCNewq3U5MCY8jonVTktbaZUZmlfzlPKz1shcVj56Jjw4PvBbG25IdKvy-2F5L74Q-2Bnzpao7XuL6QnuhiORUZgsvTNIJ0I7yJ-2FDgnxenBV0200gGDngr4XdSKAJynt0EuDdqmEZdD1o46viCvg-3D-3D" class=""&gt;Check it out here.&lt;/a&gt;&lt;/em&gt;&lt;/p&gt;&lt;p class=""&gt;.&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;.&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;.&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&lt;br class=""&gt;&amp;nbsp;&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;p style="caret-color: rgb(0, 0, 0); font-family: Helvetica; font-size: 12px; font-style: normal; font-variant-caps: normal; font-weight: normal; letter-spacing: normal; text-align: start; text-indent: 0px; text-transform: none; white-space: normal; word-spacing: 0px; -webkit-text-stroke-width: 0px; text-decoration: none;" class=""&gt;&lt;a href="http://superhuman-llc.trk.klaviyomail.com/wf/click?upn=r0bPYyJA929qYRDToey7d7uWlh9Fh01af6-2BpWZvqFCsMnHcrHzQ-2Bpt9SIuSHvs6UhopjcHwovTyItDjkuasGm1W2xo4PSzbReryDEXsNzkbxcxyeguGedXAPjf-2B2XLIiPGySs4qbGDr-2FXZjai0cX9tyOi5z0MUqG8TVoU-2FuYfkK8vHvYwKZGBEnMZPyliKrm_Texcm7ClNCJnC4QA2ERJLXnpP159NPpcVDN41ujPpklaX56IaargMptC5MvyTMihfxX9YiA0F05gPp5qdOMRMkmCdrYpCx191z0byymYYeRIBF5yTWSN5nmLQxnnvmnPNGevdqmI3q-2FSqPr7GTSXv9I-2Flrjb26fvAnBOu9GsUbwgex-2FA9TOLfboLoMuW-2Bmr5OQydIj3BwS8J-2BY4ca6-2FGBJUOQHeFItB4-2FvVsJUjh0qq-2BkED7mG3U9S4RLp6sfOq8QYO1yVhWDdNIXL1whfyXiqT5TteeLzojTBjsO-2BAtvGLJRRP2-2Bz-2B-2B51E3ypziGcZdUiS-2BboFuNIJmA-2FplSxPTYDwxL71AzAZFzxltXiPZpL0lfpvnMXR4HgCp0wzPzBYdMihPPDBAltG0tG8GmhV-2Fww-3D-3D" class=""&gt;unsubscribe&lt;/a&gt;&lt;br class=""&gt;&lt;span style="font-size: 6pt;" class=""&gt;1000 N. 1st St,&amp;nbsp;DeKalb, IL 60115&lt;/span&gt;&amp;nbsp;&lt;/p&gt;&lt;img src="http://superhuman-llc.trk.klaviyomail.com/wf/open?upn=Texcm7ClNCJnC4QA2ERJLXnpP159NPpcVDN41ujPpklaX56IaargMptC5MvyTMihfxX9YiA0F05gPp5qdOMRMkmCdrYpCx191z0byymYYeRIBF5yTWSN5nmLQxnnvmnPNGevdqmI3q-2FSqPr7GTSXv9I-2Flrjb26fvAnBOu9GsUbwgex-2FA9TOLfboLoMuW-2Bmr5OQydIj3BwS8J-2BY4ca6-2FGBChEYR1RCHsIF-2FdltgZN5UkQXRXkAX44L8iczlmQWo8eBflsiAI-2F6KfPiW4W8vO7rbmq6HOix-2BUan9xaHQLYW04RRwBICZD18-2BKIoZOt8ELb2Wskpqs9DtCLWi9AWplZh89MNB2G0EkSzGGJjIroqrbq6JjHNiEvB13pKwWaymiI2cL1vMcvyqgjLGwjgwsX5g-3D-3D" alt="" width="1" height="1" border="0" style="outline: none; text-decoration: none; caret-color: rgb(0, 0, 0); font-family: Helvetica; font-size: 12px; font-style: normal; font-variant-caps: normal; font-weight: normal; letter-spacing: normal; text-align: start; text-indent: 0px; text-transform: none; white-space: normal; word-spacing: 0px; -webkit-text-stroke-width: 0px; max-width: 550px !important; height: 1px !important; width: 1px !important; border-width: 0px !important; margin: 0px !important; padding: 0px !important;" class=""&gt;&lt;/div&gt;&lt;/blockquote&gt;&lt;/div&gt;&lt;br class=""&gt;&lt;/body&gt;&lt;/html&gt;</t>
   </si>
 </sst>
 </file>
@@ -65,8 +80,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -77,13 +93,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:B5"/>
+  <dimension ref="A2:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="2">
+      <c r="A2" t="n" s="5">
+        <v>43491.74896927083</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A2" t="n" s="4">
         <v>43491.641658148146</v>
       </c>
@@ -91,27 +115,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A2" t="n" s="3">
+    <row r="4">
+      <c r="A3" t="n" s="3">
         <v>43491.64024826389</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A3" t="n" s="2">
+    <row r="5">
+      <c r="A4" t="n" s="2">
         <v>43491.53166541667</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A4" t="n" s="1">
+    <row r="6">
+      <c r="A5" t="n" s="1">
         <v>43491.530233969905</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>